<commit_message>
Add note to documentation about S03 and S04
</commit_message>
<xml_diff>
--- a/pareto/case_studies/workshop_baseline_all_data.xlsx
+++ b/pareto/case_studies/workshop_baseline_all_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FF598E-8398-437F-9A9E-7F3CAB7D7638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3965382-1A97-42C6-8F6A-82A1C297C147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="246">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -1535,7 +1535,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1859,6 +1859,10 @@
     <xf numFmtId="3" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -5279,10 +5283,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5300,21 +5304,35 @@
       <c r="A2" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C2" s="25" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="104">
+      <c r="B3" s="135">
         <v>1</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="29"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" s="136"/>
+      <c r="C4" s="119"/>
+    </row>
+    <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="B5" s="117"/>
+      <c r="C5" s="118"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -5418,7 +5436,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -17952,7 +17970,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -18567,7 +18585,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add subsurface risk data to workshop_baseline_all_data.xlsx and fix tests
</commit_message>
<xml_diff>
--- a/pareto/case_studies/workshop_baseline_all_data.xlsx
+++ b/pareto/case_studies/workshop_baseline_all_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62D072A-EEFB-43BC-A0FE-EDC6764271FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A5ADF4-9514-40C3-9AD8-C89FA4E65423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="266">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -1629,7 +1629,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1978,6 +1978,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="47" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3016,20 +3019,45 @@
   <sheetPr>
     <tabColor theme="1" tint="0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="145" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3042,20 +3070,45 @@
   <sheetPr>
     <tabColor theme="1" tint="0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="15.140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="145" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="29">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.65</v>
       </c>
     </row>
   </sheetData>
@@ -3068,20 +3121,45 @@
   <sheetPr>
     <tabColor theme="1" tint="0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="145" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="29">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.27</v>
       </c>
     </row>
   </sheetData>
@@ -3094,20 +3172,45 @@
   <sheetPr>
     <tabColor theme="1" tint="0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="13" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="145" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="29">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>
@@ -3120,20 +3223,45 @@
   <sheetPr>
     <tabColor theme="1" tint="0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="145" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="29">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="9">
+        <v>5.46</v>
       </c>
     </row>
   </sheetData>
@@ -3146,20 +3274,45 @@
   <sheetPr>
     <tabColor theme="1" tint="0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="13.28515625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="145" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="29">
+        <v>3.03</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="9">
+        <v>4.1900000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -3172,20 +3325,45 @@
   <sheetPr>
     <tabColor theme="1" tint="0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="13.5703125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="145" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="29">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve units support for emissions calculations
</commit_message>
<xml_diff>
--- a/pareto/case_studies/workshop_baseline_all_data.xlsx
+++ b/pareto/case_studies/workshop_baseline_all_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3194126B-32D6-4B8C-B044-2D6C3236B900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65010237-EC1C-42FE-97EB-49F1ADC02CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" firstSheet="93" activeTab="95" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="278">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -983,21 +983,6 @@
   </si>
   <si>
     <t>PM 2.5</t>
-  </si>
-  <si>
-    <t>Trucking (g/hour)</t>
-  </si>
-  <si>
-    <t>Pipeline Operations (g/(bbl-mile))</t>
-  </si>
-  <si>
-    <t>Pipeline Installation (g/mile)</t>
-  </si>
-  <si>
-    <t>Disposal (g/bbl)</t>
-  </si>
-  <si>
-    <t>Storage (g/bbl-week)</t>
   </si>
 </sst>
 </file>
@@ -2496,7 +2481,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3056,9 +3041,7 @@
   </sheetPr>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5848,7 +5831,7 @@
   <dimension ref="A1:BB12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -20597,8 +20580,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>278</v>
+      <c r="A3" s="26" t="str">
+        <f>_xlfn.CONCAT("Trucking [", VLOOKUP("mass", Units!A2:B12, 2, FALSE), "/hour]")</f>
+        <v>Trucking [g/hour]</v>
       </c>
       <c r="B3" s="146">
         <v>2035000</v>
@@ -20617,8 +20601,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>279</v>
+      <c r="A4" s="26" t="str">
+        <f>_xlfn.CONCAT("Pipeline Operations [", VLOOKUP("mass", Units!A2:B12, 2, FALSE), "/(", VLOOKUP("volume", Units!A2:B12, 2, FALSE), "*", VLOOKUP("distance", Units!A2:B12, 2, FALSE), ")]")</f>
+        <v>Pipeline Operations [g/(bbl*mile)]</v>
       </c>
       <c r="B4" s="146">
         <v>22</v>
@@ -20637,8 +20622,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>280</v>
+      <c r="A5" s="26" t="str">
+        <f>_xlfn.CONCAT("Pipeline Installation [", VLOOKUP("mass", Units!A2:B12, 2, FALSE), "/", VLOOKUP("distance", Units!A2:B12, 2, FALSE), "]")</f>
+        <v>Pipeline Installation [g/mile]</v>
       </c>
       <c r="B5" s="146">
         <v>310000000</v>
@@ -20657,8 +20643,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>281</v>
+      <c r="A6" s="26" t="str">
+        <f>_xlfn.CONCAT("Disposal [", VLOOKUP("mass", Units!A2:B12, 2, FALSE), "/", VLOOKUP("volume", Units!A2:B12, 2, FALSE), "]")</f>
+        <v>Disposal [g/bbl]</v>
       </c>
       <c r="B6" s="146">
         <v>970</v>
@@ -20677,8 +20664,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27" t="s">
-        <v>282</v>
+      <c r="A7" s="27" t="str">
+        <f>_xlfn.CONCAT("Storage [", VLOOKUP("mass", Units!A2:B12, 2, FALSE), "/(", VLOOKUP("volume", Units!A2:B12, 2, FALSE), "*", VLOOKUP("decision period", Units!A2:B12, 2, FALSE), ")]")</f>
+        <v>Storage [g/(bbl*week)]</v>
       </c>
       <c r="B7" s="148">
         <v>1000</v>
@@ -20708,7 +20696,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -20719,8 +20707,8 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Air Emissions Coefficients  for Treatment Technologies [emissions/volume time]")</f>
-        <v>Table of Air Emissions Coefficients  for Treatment Technologies [emissions/volume time]</v>
+        <f>_xlfn.CONCAT("Table of Air Emissions Coefficients for Treatment Technologies [", VLOOKUP("mass", Units!A2:B12, 2, FALSE), "/", VLOOKUP("volume", Units!A2:B12, 2, FALSE), "]")</f>
+        <v>Table of Air Emissions Coefficients for Treatment Technologies [g/bbl]</v>
       </c>
       <c r="B1" s="1"/>
     </row>

</xml_diff>